<commit_message>
new table and always dhcp
</commit_message>
<xml_diff>
--- a/host/function/scripts/IA-xx.xlsx
+++ b/host/function/scripts/IA-xx.xlsx
@@ -13,17 +13,17 @@
   <calcPr calcOnSave="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1596475201" val="976" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1596475201" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1596475201" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1596475201"/>
+      <pm:revision xmlns:pm="smNativeData" day="1596743202" val="976" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1596743202" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1596743202" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1596743202"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="37">
   <si>
     <t>BBB_IP</t>
   </si>
@@ -98,6 +98,42 @@
   </si>
   <si>
     <t>1,2,3</t>
+  </si>
+  <si>
+    <t>10.128.102.104</t>
+  </si>
+  <si>
+    <t>BBB-PS-DCLink</t>
+  </si>
+  <si>
+    <t>PowerSupply</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,2 </t>
+  </si>
+  <si>
+    <t>FBP-DCLink</t>
+  </si>
+  <si>
+    <t>10.128.102.122</t>
+  </si>
+  <si>
+    <t>BBB-SI-CORRETORAS1</t>
+  </si>
+  <si>
+    <t>1,2,3,4,5,6,7</t>
+  </si>
+  <si>
+    <t>CH1,CH2,CV1,CV2,CH3,CH4,CV3</t>
+  </si>
+  <si>
+    <t>10.128.102.132</t>
+  </si>
+  <si>
+    <t>BBB-SI-CORRETORAS2</t>
+  </si>
+  <si>
+    <t>CV4,CH5,CH6,CV5,CV6,CH7,CV7</t>
   </si>
 </sst>
 </file>
@@ -123,7 +159,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1596475201" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1596743202" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -138,7 +174,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1596475201" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1596743202" ulstyle="none" kern="1">
             <pm:latin face="Basic Sans" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -154,7 +190,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1596475201" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1596743202" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default" weight="bold"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -176,7 +212,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1596475201" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1596743202" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -198,7 +234,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1596475201"/>
+          <pm:border xmlns:pm="smNativeData" id="1596743202"/>
         </ext>
       </extLst>
     </border>
@@ -217,7 +253,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1596475201"/>
+          <pm:border xmlns:pm="smNativeData" id="1596743202"/>
         </ext>
       </extLst>
     </border>
@@ -239,10 +275,10 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1596475201" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1596743202" count="1">
         <pm:charStyle name="Normal" fontId="0"/>
       </pm:charStyles>
-      <pm:colors xmlns:pm="smNativeData" id="1596475201" count="5">
+      <pm:colors xmlns:pm="smNativeData" id="1596743202" count="5">
         <pm:color name="Color 24" rgb="95B3D7"/>
         <pm:color name="Color 25" rgb="DCE6F1"/>
         <pm:color name="Color 26" rgb="D8D8D8"/>
@@ -513,7 +549,7 @@
   <dimension ref="A1:XFD12"/>
   <sheetViews>
     <sheetView tabSelected="1" view="normal" zoomScale="175" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="12.90"/>
@@ -522,7 +558,7 @@
     <col min="2" max="2" width="38.702703" customWidth="1" style="1"/>
     <col min="3" max="3" width="15.765766" customWidth="1" style="1"/>
     <col min="4" max="4" width="10.801802" customWidth="1" style="1"/>
-    <col min="5" max="5" width="15.045045" customWidth="1" style="1"/>
+    <col min="5" max="5" width="29.558559" customWidth="1" style="1"/>
     <col min="6" max="6" width="15.000000" customWidth="1" style="1"/>
     <col min="7" max="16384" width="10.000000" style="1"/>
   </cols>
@@ -629,11 +665,62 @@
         <v>24</v>
       </c>
     </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1596475201" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1596743202" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -642,14 +729,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1596475201" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1596475201" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1596743202" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1596743202" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1596475201" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1596743202" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>